<commit_message>
Added pid list csvs
</commit_message>
<xml_diff>
--- a/PID LISTS/S50.xlsx
+++ b/PID LISTS/S50.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\MQB TUning\PID Lists\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Documents\YakTuner\PID LISTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{17106E19-575E-41F7-8940-E9962A211F1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD5879E6-A559-47BD-9BA1-ABE254914755}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" activeTab="2"/>
+    <workbookView xWindow="9315" yWindow="0" windowWidth="29205" windowHeight="15015" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WG" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="86">
   <si>
     <t>%01.1f</t>
   </si>
@@ -241,12 +241,51 @@
   </si>
   <si>
     <t>kpa</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>Equation</t>
+  </si>
+  <si>
+    <t>Format</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>Signed</t>
+  </si>
+  <si>
+    <t>ProgMin</t>
+  </si>
+  <si>
+    <t>ProgMax</t>
+  </si>
+  <si>
+    <t>WarnMin</t>
+  </si>
+  <si>
+    <t>WarnMax</t>
+  </si>
+  <si>
+    <t>Smoothing</t>
+  </si>
+  <si>
+    <t>Enabled</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1080,11 +1119,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection sqref="A1:M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1094,60 +1133,60 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>74</v>
       </c>
       <c r="C1" t="s">
-        <v>21</v>
+        <v>75</v>
       </c>
       <c r="D1" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
       <c r="E1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F1">
-        <v>2</v>
-      </c>
-      <c r="G1" t="b">
-        <v>0</v>
-      </c>
-      <c r="H1">
-        <v>0</v>
-      </c>
-      <c r="I1">
-        <v>100</v>
-      </c>
-      <c r="J1">
-        <v>-10</v>
-      </c>
-      <c r="K1">
-        <v>500</v>
-      </c>
-      <c r="L1">
-        <v>0</v>
-      </c>
-      <c r="M1" t="b">
-        <v>1</v>
+        <v>77</v>
+      </c>
+      <c r="F1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H1" t="s">
+        <v>80</v>
+      </c>
+      <c r="I1" t="s">
+        <v>81</v>
+      </c>
+      <c r="J1" t="s">
+        <v>82</v>
+      </c>
+      <c r="K1" t="s">
+        <v>83</v>
+      </c>
+      <c r="L1" t="s">
+        <v>84</v>
+      </c>
+      <c r="M1" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="F2">
         <v>2</v>
@@ -1159,13 +1198,13 @@
         <v>0</v>
       </c>
       <c r="I2">
-        <v>7000</v>
+        <v>100</v>
       </c>
       <c r="J2">
-        <v>-1</v>
+        <v>-10</v>
       </c>
       <c r="K2">
-        <v>10000</v>
+        <v>500</v>
       </c>
       <c r="L2">
         <v>0</v>
@@ -1176,16 +1215,19 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="F3">
         <v>2</v>
@@ -1197,13 +1239,13 @@
         <v>0</v>
       </c>
       <c r="I3">
-        <v>2</v>
+        <v>7000</v>
       </c>
       <c r="J3">
         <v>-1</v>
       </c>
       <c r="K3">
-        <v>10</v>
+        <v>10000</v>
       </c>
       <c r="L3">
         <v>0</v>
@@ -1214,7 +1256,7 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
         <v>26</v>
@@ -1223,7 +1265,7 @@
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F4">
         <v>2</v>
@@ -1238,10 +1280,10 @@
         <v>2</v>
       </c>
       <c r="J4">
-        <v>-1000</v>
+        <v>-1</v>
       </c>
       <c r="K4">
-        <v>1000</v>
+        <v>10</v>
       </c>
       <c r="L4">
         <v>0</v>
@@ -1252,19 +1294,16 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B5" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="C5" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="D5" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E5" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="F5">
         <v>2</v>
@@ -1276,7 +1315,7 @@
         <v>0</v>
       </c>
       <c r="I5">
-        <v>100</v>
+        <v>2</v>
       </c>
       <c r="J5">
         <v>-1000</v>
@@ -1293,19 +1332,19 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B6" t="s">
-        <v>72</v>
+        <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="D6" t="s">
         <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="F6">
         <v>2</v>
@@ -1317,13 +1356,13 @@
         <v>0</v>
       </c>
       <c r="I6">
-        <v>320</v>
+        <v>100</v>
       </c>
       <c r="J6">
-        <v>-1</v>
+        <v>-1000</v>
       </c>
       <c r="K6">
-        <v>350</v>
+        <v>1000</v>
       </c>
       <c r="L6">
         <v>0</v>
@@ -1334,22 +1373,22 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B7" t="s">
         <v>72</v>
       </c>
       <c r="C7" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="D7" t="s">
         <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="F7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G7" t="b">
         <v>0</v>
@@ -1375,19 +1414,22 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>54</v>
+        <v>47</v>
+      </c>
+      <c r="B8" t="s">
+        <v>72</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="D8" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E8" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="F8">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G8" t="b">
         <v>0</v>
@@ -1396,13 +1438,13 @@
         <v>0</v>
       </c>
       <c r="I8">
-        <v>1</v>
+        <v>320</v>
       </c>
       <c r="J8">
-        <v>-1000</v>
+        <v>-1</v>
       </c>
       <c r="K8">
-        <v>1000</v>
+        <v>350</v>
       </c>
       <c r="L8">
         <v>0</v>
@@ -1413,22 +1455,19 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>58</v>
-      </c>
-      <c r="B9" t="s">
-        <v>4</v>
+        <v>54</v>
       </c>
       <c r="C9" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="D9" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E9" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G9" t="b">
         <v>0</v>
@@ -1437,7 +1476,7 @@
         <v>0</v>
       </c>
       <c r="I9">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="J9">
         <v>-1000</v>
@@ -1454,7 +1493,7 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B10" t="s">
         <v>4</v>
@@ -1466,7 +1505,7 @@
         <v>0</v>
       </c>
       <c r="E10" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="F10">
         <v>2</v>
@@ -1495,19 +1534,22 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>49</v>
+        <v>56</v>
+      </c>
+      <c r="B11" t="s">
+        <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="D11" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E11" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="F11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G11" t="b">
         <v>0</v>
@@ -1516,7 +1558,7 @@
         <v>0</v>
       </c>
       <c r="I11">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="J11">
         <v>-1000</v>
@@ -1528,6 +1570,44 @@
         <v>0</v>
       </c>
       <c r="M11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" t="s">
+        <v>50</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12" t="b">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>-1000</v>
+      </c>
+      <c r="K12">
+        <v>1000</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1537,11 +1617,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection sqref="A1:M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1551,48 +1631,51 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>73</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>74</v>
       </c>
       <c r="C1" t="s">
-        <v>11</v>
+        <v>75</v>
       </c>
       <c r="D1" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
       <c r="E1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1">
-        <v>2</v>
-      </c>
-      <c r="G1" t="b">
-        <v>0</v>
-      </c>
-      <c r="H1">
-        <v>0</v>
-      </c>
-      <c r="I1">
-        <v>7000</v>
-      </c>
-      <c r="J1">
-        <v>-1</v>
-      </c>
-      <c r="K1">
-        <v>10000</v>
-      </c>
-      <c r="L1">
-        <v>0</v>
-      </c>
-      <c r="M1" t="b">
-        <v>1</v>
+        <v>77</v>
+      </c>
+      <c r="F1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H1" t="s">
+        <v>80</v>
+      </c>
+      <c r="I1" t="s">
+        <v>81</v>
+      </c>
+      <c r="J1" t="s">
+        <v>82</v>
+      </c>
+      <c r="K1" t="s">
+        <v>83</v>
+      </c>
+      <c r="L1" t="s">
+        <v>84</v>
+      </c>
+      <c r="M1" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
       </c>
       <c r="C2" t="s">
         <v>11</v>
@@ -1601,10 +1684,10 @@
         <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G2" t="b">
         <v>0</v>
@@ -1613,13 +1696,13 @@
         <v>0</v>
       </c>
       <c r="I2">
-        <v>6</v>
+        <v>7000</v>
       </c>
       <c r="J2">
-        <v>-1000</v>
+        <v>-1</v>
       </c>
       <c r="K2">
-        <v>1000</v>
+        <v>10000</v>
       </c>
       <c r="L2">
         <v>0</v>
@@ -1630,34 +1713,34 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3" t="b">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
         <v>6</v>
       </c>
-      <c r="D3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3">
-        <v>2</v>
-      </c>
-      <c r="G3" t="b">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>0.75</v>
-      </c>
-      <c r="I3">
-        <v>1.25</v>
-      </c>
       <c r="J3">
-        <v>-100</v>
+        <v>-1000</v>
       </c>
       <c r="K3">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="L3">
         <v>0</v>
@@ -1668,16 +1751,16 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>60</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="D4" t="s">
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>62</v>
+        <v>7</v>
       </c>
       <c r="F4">
         <v>2</v>
@@ -1706,28 +1789,28 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>60</v>
       </c>
       <c r="C5" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="D5" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E5" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="F5">
         <v>2</v>
       </c>
       <c r="G5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H5">
-        <v>-1</v>
+        <v>0.75</v>
       </c>
       <c r="I5">
-        <v>1</v>
+        <v>1.25</v>
       </c>
       <c r="J5">
         <v>-100</v>
@@ -1744,37 +1827,34 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B6" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="C6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D6" t="s">
         <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F6">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I6">
-        <v>320</v>
+        <v>1</v>
       </c>
       <c r="J6">
-        <v>-1</v>
+        <v>-100</v>
       </c>
       <c r="K6">
-        <v>350</v>
+        <v>100</v>
       </c>
       <c r="L6">
         <v>0</v>
@@ -1785,34 +1865,37 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>63</v>
+        <v>41</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>64</v>
+        <v>42</v>
       </c>
       <c r="D7" t="s">
         <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>65</v>
+        <v>43</v>
       </c>
       <c r="F7">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H7">
-        <v>-50</v>
+        <v>0</v>
       </c>
       <c r="I7">
-        <v>50</v>
+        <v>320</v>
       </c>
       <c r="J7">
-        <v>-100</v>
+        <v>-1</v>
       </c>
       <c r="K7">
-        <v>100</v>
+        <v>350</v>
       </c>
       <c r="L7">
         <v>0</v>
@@ -1823,34 +1906,34 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>64</v>
       </c>
       <c r="D8" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8">
-        <v>0</v>
+        <v>-50</v>
       </c>
       <c r="I8">
-        <v>4</v>
+        <v>50</v>
       </c>
       <c r="J8">
-        <v>-1000</v>
+        <v>-100</v>
       </c>
       <c r="K8">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="L8">
         <v>0</v>
@@ -1861,34 +1944,34 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C9" t="s">
-        <v>69</v>
+        <v>11</v>
       </c>
       <c r="D9" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E9" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H9">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="I9">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J9">
-        <v>-100</v>
+        <v>-1000</v>
       </c>
       <c r="K9">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="L9">
         <v>0</v>
@@ -1899,28 +1982,28 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>68</v>
       </c>
       <c r="C10" t="s">
-        <v>11</v>
+        <v>69</v>
       </c>
       <c r="D10" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E10" t="s">
-        <v>19</v>
+        <v>70</v>
       </c>
       <c r="F10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I10">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="J10">
         <v>-100</v>
@@ -1932,6 +2015,44 @@
         <v>0</v>
       </c>
       <c r="M10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11" t="b">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>26</v>
+      </c>
+      <c r="J11">
+        <v>-100</v>
+      </c>
+      <c r="K11">
+        <v>100</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1941,11 +2062,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+      <selection sqref="A1:M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1955,64 +2076,64 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>73</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>74</v>
       </c>
       <c r="C1" t="s">
-        <v>11</v>
+        <v>75</v>
       </c>
       <c r="D1" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
       <c r="E1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1">
-        <v>2</v>
-      </c>
-      <c r="G1" t="b">
-        <v>0</v>
-      </c>
-      <c r="H1">
-        <v>0</v>
-      </c>
-      <c r="I1">
-        <v>7000</v>
-      </c>
-      <c r="J1">
-        <v>-1</v>
-      </c>
-      <c r="K1">
-        <v>10000</v>
-      </c>
-      <c r="L1">
-        <v>0</v>
-      </c>
-      <c r="M1" t="b">
-        <v>1</v>
+        <v>77</v>
+      </c>
+      <c r="F1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H1" t="s">
+        <v>80</v>
+      </c>
+      <c r="I1" t="s">
+        <v>81</v>
+      </c>
+      <c r="J1" t="s">
+        <v>82</v>
+      </c>
+      <c r="K1" t="s">
+        <v>83</v>
+      </c>
+      <c r="L1" t="s">
+        <v>84</v>
+      </c>
+      <c r="M1" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
       <c r="G2" t="b">
         <v>0</v>
       </c>
@@ -2020,13 +2141,13 @@
         <v>0</v>
       </c>
       <c r="I2">
-        <v>-5</v>
+        <v>7000</v>
       </c>
       <c r="J2">
-        <v>-5</v>
+        <v>-1</v>
       </c>
       <c r="K2">
-        <v>1</v>
+        <v>10000</v>
       </c>
       <c r="L2">
         <v>0</v>
@@ -2037,7 +2158,7 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>71</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -2049,7 +2170,7 @@
         <v>3</v>
       </c>
       <c r="E3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -2078,7 +2199,7 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
@@ -2090,7 +2211,7 @@
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -2119,7 +2240,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>
@@ -2131,7 +2252,7 @@
         <v>3</v>
       </c>
       <c r="E5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -2160,42 +2281,83 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6" t="b">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>-5</v>
+      </c>
+      <c r="J6">
+        <v>-5</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>13</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>14</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" t="s">
         <v>15</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D7" t="s">
         <v>8</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E7" t="s">
         <v>16</v>
       </c>
-      <c r="F6">
+      <c r="F7">
         <v>4</v>
       </c>
-      <c r="G6" t="b">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
+      <c r="G7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
         <v>2000</v>
       </c>
-      <c r="J6">
+      <c r="J7">
         <v>-100</v>
       </c>
-      <c r="K6">
+      <c r="K7">
         <v>50000</v>
       </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
-      <c r="M6" t="b">
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>